<commit_message>
add template pop gratis
</commit_message>
<xml_diff>
--- a/Template POP Coret Harga.xlsx
+++ b/Template POP Coret Harga.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Programming\Web\pop-maker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pindahan\Jalal\Programming\WEB\Mail Merge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F48DDF-6619-4DDE-8C19-662BC9AA53FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C41F9AC-ECC9-40FF-92B0-5879115F5C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>KODE</t>
   </si>
@@ -67,6 +59,12 @@
   </si>
   <si>
     <t>30/11/2024</t>
+  </si>
+  <si>
+    <t>CATATAN</t>
+  </si>
+  <si>
+    <t>PRODUK DENGAN TANDA KHUSUS</t>
   </si>
 </sst>
 </file>
@@ -135,18 +133,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -455,26 +450,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,12 +501,15 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1234567890</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2">
@@ -523,240 +522,99 @@
       <c r="E2" s="2">
         <v>9000</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="str">
-        <f t="shared" ref="H2:H20" si="0">LEFT(B2, FIND(" ", B2&amp; " ") - 1)</f>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2" si="0">LEFT(B2, FIND(" ", B2&amp; " ") - 1)</f>
         <v>MAKUKU</v>
       </c>
-      <c r="I2" s="5" t="str">
-        <f t="shared" ref="I2:I20" si="1">TRIM(LEFT(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2)), FIND("×", SUBSTITUTE(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2)), " ", "×", LEN(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2))) - LEN(SUBSTITUTE(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2)), " ", "")))) - 1))</f>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2" si="1">TRIM(LEFT(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2)), FIND("×", SUBSTITUTE(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2)), " ", "×", LEN(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2))) - LEN(SUBSTITUTE(MID(B2, FIND(" ", B2) + 1, LEN(B2) - FIND(" ", B2)), " ", "")))) - 1))</f>
         <v>BRONZE PANTS</v>
       </c>
-      <c r="J2" s="5" t="str">
-        <f t="shared" ref="J2:J20" si="2">TRIM(RIGHT(SUBSTITUTE(B2, " ", REPT(" ", 100)),100))</f>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2" si="2">TRIM(RIGHT(SUBSTITUTE(B2, " ", REPT(" ", 100)),100))</f>
         <v>S56</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="6:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>